<commit_message>
Added: logger. Updated: processes excel file
</commit_message>
<xml_diff>
--- a/processes.xlsx
+++ b/processes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebastian.villegasz\Documents\Personal\judicial-processes-scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F98AC3E-9DC5-4F66-A2BA-839E0C605CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265C4A21-91C4-471A-9610-7E5F171B425A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{881731EB-258D-47D9-AE5D-C7DBBFC25984}"/>
   </bookViews>
@@ -1455,19 +1455,19 @@
     <t>05001310301720190015501</t>
   </si>
   <si>
-    <t>17 REVISARLO EN TRIBUNAL</t>
-  </si>
-  <si>
     <t>05001310301920200017001</t>
   </si>
   <si>
-    <t>19 Revisarlo en Tribunales</t>
-  </si>
-  <si>
-    <t>15 REVISARLO EN TRIBUNAL</t>
-  </si>
-  <si>
     <t>05001310301520210005601</t>
+  </si>
+  <si>
+    <t>17 TRIBUNAL SUPERIOR DE MEDELLIN</t>
+  </si>
+  <si>
+    <t>15 TRIBUNAL SUPERIOR DE MEDELLIN</t>
+  </si>
+  <si>
+    <t>19 TRIBUNAL SUPERIOR DE MEDELLIN</t>
   </si>
 </sst>
 </file>
@@ -1822,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3476A290-B83E-4AAC-8AE2-6644A5F070CB}">
   <dimension ref="A1:C192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1948,7 +1948,7 @@
         <v>472</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C11" t="s">
         <v>147</v>
@@ -2231,10 +2231,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C37" t="s">
         <v>89</v>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>476</v>

</xml_diff>